<commit_message>
cost timeseries for generation added in the model
</commit_message>
<xml_diff>
--- a/testcases/SP53224_10020195_87729.xlsx
+++ b/testcases/SP53224_10020195_87729.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="bus" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,6 +18,7 @@
     <sheet name="timeseries" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="EVs" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="EVsTravelDiary" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="timeseriesGen" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="193">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -606,6 +607,9 @@
   <si>
     <t xml:space="preserve">EEnd</t>
   </si>
+  <si>
+    <t xml:space="preserve">cost(pounds/kwh)</t>
+  </si>
 </sst>
 </file>
 
@@ -724,7 +728,7 @@
   <dimension ref="A1:I77"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="146:164 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2984,12 +2988,12 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="1" sqref="146:164 E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.67"/>
   </cols>
   <sheetData>
@@ -3085,6 +3089,1628 @@
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C145"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A130" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A164" activeCellId="0" sqref="146:164"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C68" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C69" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C70" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C71" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C72" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C74" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C75" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C76" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C81" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C84" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C85" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C86" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C87" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C88" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C89" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C90" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C91" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C92" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C93" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C94" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C95" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C96" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C97" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C98" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C99" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C100" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C101" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C102" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C103" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C104" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C105" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C106" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C107" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C108" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C109" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C110" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C111" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C112" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C113" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C114" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C115" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C116" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C117" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C118" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C119" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="n">
+        <v>118</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C120" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="n">
+        <v>119</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C121" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C122" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="n">
+        <v>121</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C123" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="B124" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C124" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="B125" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C125" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="B126" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C126" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="n">
+        <v>125</v>
+      </c>
+      <c r="B127" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C127" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C128" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C129" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C130" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C131" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C132" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C133" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C134" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C135" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C136" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C137" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C138" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C139" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="n">
+        <v>138</v>
+      </c>
+      <c r="B140" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C140" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C141" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C142" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="n">
+        <v>141</v>
+      </c>
+      <c r="B143" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C143" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C144" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C145" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -3097,7 +4723,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="146:164 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3604,7 +5230,7 @@
   <dimension ref="A1:M75"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="1" sqref="146:164 F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6706,7 +8332,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W27" activeCellId="0" sqref="W27"/>
+      <selection pane="topLeft" activeCell="W27" activeCellId="1" sqref="146:164 W27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6845,7 +8471,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T28" activeCellId="0" sqref="T28"/>
+      <selection pane="topLeft" activeCell="T28" activeCellId="1" sqref="146:164 T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6888,8 +8514,8 @@
   </sheetPr>
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V7" activeCellId="0" sqref="V7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="146:164 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7076,7 +8702,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W37" activeCellId="0" sqref="W37"/>
+      <selection pane="topLeft" activeCell="W37" activeCellId="1" sqref="146:164 W37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7113,7 +8739,7 @@
   <dimension ref="A1:X145"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="146:164 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17870,7 +19496,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U24" activeCellId="0" sqref="U24"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="146:164 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>